<commit_message>
add session time schedule
</commit_message>
<xml_diff>
--- a/src/models/data/time_schedule.xlsx
+++ b/src/models/data/time_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EDA5ED-41C1-400C-8700-9B2681E4E44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7B57A5-6E9E-43C3-A9D6-30B9DB54DB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="19224" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>time_start</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>6e5a0a9a-6794-4127-bf5c-4927bc7d2279</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Afternoon</t>
   </si>
 </sst>
 </file>
@@ -471,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,7 +499,7 @@
     <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -500,8 +509,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -511,8 +523,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -522,8 +537,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -533,8 +551,11 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -544,8 +565,11 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -555,8 +579,11 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -566,8 +593,11 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -577,8 +607,11 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -588,8 +621,11 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -599,8 +635,11 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -610,8 +649,11 @@
       <c r="C11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -621,8 +663,11 @@
       <c r="C12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -632,8 +677,11 @@
       <c r="C13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -643,8 +691,11 @@
       <c r="C14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -654,8 +705,11 @@
       <c r="C15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -665,8 +719,11 @@
       <c r="C16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -675,6 +732,9 @@
       </c>
       <c r="C17" t="s">
         <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>